<commit_message>
Get test set working with loss model included
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C2B20E-376B-4F2F-85BC-FB6069F94E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48033E2-7395-4834-8584-ECD26FDDD6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" firstSheet="3" activeTab="7" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcox" sheetId="3" r:id="rId1"/>
@@ -1641,7 +1641,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2194,7 @@
         <v>43905</v>
       </c>
       <c r="D29" s="2">
-        <v>44114</v>
+        <v>44115</v>
       </c>
       <c r="E29" s="2">
         <v>44360</v>
@@ -2308,7 +2308,7 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
@@ -2326,7 +2326,7 @@
         <v>158</v>
       </c>
       <c r="C36">
-        <v>37.299999999999997</v>
+        <v>3.5</v>
       </c>
       <c r="D36">
         <v>37.299999999999997</v>
@@ -2380,7 +2380,7 @@
         <v>41</v>
       </c>
       <c r="C39">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D39">
         <v>86</v>
@@ -2398,7 +2398,7 @@
         <v>42</v>
       </c>
       <c r="C40" s="2">
-        <v>44360</v>
+        <v>44115</v>
       </c>
       <c r="D40" s="2">
         <v>44360</v>
@@ -2416,7 +2416,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -2434,7 +2434,7 @@
         <v>44</v>
       </c>
       <c r="C42" s="2">
-        <v>44578</v>
+        <v>44206</v>
       </c>
       <c r="D42" s="2">
         <v>44578</v>
@@ -2452,7 +2452,7 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -2470,7 +2470,7 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
         <v>22</v>
@@ -9283,11 +9283,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27FB4FB-42CF-4046-81E6-EAE466E39234}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:F4"/>
+      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10019,7 +10019,7 @@
         <v>45026</v>
       </c>
       <c r="F40" s="2">
-        <v>45074</v>
+        <v>45166</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -10233,7 +10233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B09E1-BD11-449B-8251-3F1E868B35B7}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Fix crop name in test configs
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48033E2-7395-4834-8584-ECD26FDDD6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1B4521-0F10-40B8-9238-14ADEDB8A1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-5925" windowWidth="16440" windowHeight="28440" firstSheet="3" activeTab="7" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcox" sheetId="3" r:id="rId1"/>
@@ -526,9 +526,6 @@
     <t>Figures in red uncertain or are guesses.</t>
   </si>
   <si>
-    <t>Carrot Vegetable General</t>
-  </si>
-  <si>
     <t>Some</t>
   </si>
   <si>
@@ -773,6 +770,9 @@
   </si>
   <si>
     <t>FollowingFieldYield</t>
+  </si>
+  <si>
+    <t>Carrot Vegetable Processing</t>
   </si>
 </sst>
 </file>
@@ -1660,16 +1660,16 @@
         <v>62</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>113</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>114</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -1687,16 +1687,16 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1720,43 +1720,43 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1897,10 +1897,10 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" t="s">
         <v>64</v>
@@ -1909,7 +1909,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>44</v>
@@ -2094,16 +2094,16 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" t="s">
         <v>64</v>
       </c>
       <c r="F24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -2116,7 +2116,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>3.5</v>
@@ -2308,13 +2308,13 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" t="s">
         <v>26</v>
@@ -2323,7 +2323,7 @@
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>3.5</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="54" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
@@ -2624,16 +2624,16 @@
         <v>62</v>
       </c>
       <c r="C1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>118</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -2654,16 +2654,16 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2687,43 +2687,43 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2879,7 +2879,7 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14">
         <v>65</v>
@@ -3089,7 +3089,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>56.5</v>
@@ -3300,7 +3300,7 @@
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>70.599999999999994</v>
@@ -3510,7 +3510,7 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="39"/>
       <c r="D51" s="6"/>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -3617,8 +3617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,16 +3637,16 @@
         <v>62</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>122</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -3667,16 +3667,16 @@
         <v>48</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -3700,43 +3700,43 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17">
         <v>0</v>
@@ -3850,7 +3850,7 @@
         <v>67</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>67</v>
@@ -3880,10 +3880,10 @@
         <v>64</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>64</v>
@@ -3892,7 +3892,7 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>50</v>
@@ -4077,10 +4077,10 @@
         <v>25</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>64</v>
@@ -4102,7 +4102,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>30.4</v>
@@ -4298,7 +4298,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="D35" s="17" t="s">
         <v>64</v>
@@ -4307,13 +4307,13 @@
         <v>64</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="17">
         <v>82.5</v>
@@ -4630,19 +4630,19 @@
         <v>62</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>126</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>127</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -4663,19 +4663,19 @@
         <v>48</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -4702,49 +4702,49 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17">
         <v>0</v>
@@ -4879,7 +4879,7 @@
         <v>67</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" s="27" t="s">
         <v>67</v>
@@ -4906,7 +4906,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>26</v>
@@ -4915,16 +4915,16 @@
         <v>70</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>16.600000000000001</v>
@@ -5145,7 +5145,7 @@
         <v>70</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>64</v>
@@ -5167,7 +5167,7 @@
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="17">
         <v>33</v>
@@ -5396,13 +5396,13 @@
         <v>70</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>64</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G35" s="16" t="s">
         <v>70</v>
@@ -5411,7 +5411,7 @@
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="17">
         <v>19</v>
@@ -5758,16 +5758,16 @@
         <v>62</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>131</v>
       </c>
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
@@ -5788,16 +5788,16 @@
         <v>48</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -5821,43 +5821,43 @@
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17">
         <v>0</v>
@@ -5968,7 +5968,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>67</v>
@@ -5998,7 +5998,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>26</v>
@@ -6007,13 +6007,13 @@
         <v>64</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="17">
         <v>10</v>
@@ -6204,7 +6204,7 @@
         <v>64</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>26</v>
@@ -6223,7 +6223,7 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="17">
         <v>74.099999999999994</v>
@@ -6422,19 +6422,19 @@
         <v>64</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E35" s="17" t="s">
         <v>26</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="17">
         <v>70.7</v>
@@ -6645,7 +6645,7 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="24"/>
@@ -6683,7 +6683,7 @@
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
@@ -6702,7 +6702,7 @@
     </row>
     <row r="54" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -6756,22 +6756,22 @@
         <v>62</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>137</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -6792,22 +6792,22 @@
         <v>48</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -6837,55 +6837,55 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17">
         <v>0</v>
@@ -7068,28 +7068,28 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>103</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>10</v>
@@ -7269,7 +7269,7 @@
         <v>54</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>54</v>
@@ -7334,22 +7334,22 @@
         <v>25</v>
       </c>
       <c r="C24" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -7365,7 +7365,7 @@
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="17">
         <v>81.900000000000006</v>
@@ -7543,7 +7543,7 @@
         <v>54</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>54</v>
@@ -7621,28 +7621,28 @@
         <v>37</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="G35" s="17" t="s">
-        <v>105</v>
-      </c>
       <c r="H35" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="17">
         <v>15.3</v>
@@ -7817,7 +7817,7 @@
         <v>54</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>54</v>
@@ -7914,7 +7914,7 @@
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
@@ -7935,7 +7935,7 @@
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="24"/>
@@ -8029,22 +8029,22 @@
         <v>62</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>142</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>143</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -8065,22 +8065,22 @@
         <v>48</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -8110,55 +8110,55 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="17">
         <v>0</v>
@@ -8341,28 +8341,28 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>12.3</v>
@@ -8607,22 +8607,22 @@
         <v>25</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -8638,7 +8638,7 @@
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25" s="17">
         <v>17.2</v>
@@ -8894,28 +8894,28 @@
         <v>37</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36" s="17">
         <v>12.3</v>
@@ -9187,7 +9187,7 @@
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
@@ -9208,7 +9208,7 @@
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="24"/>
@@ -9248,7 +9248,7 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
@@ -9284,10 +9284,10 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomRight" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9303,13 +9303,13 @@
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9353,43 +9353,43 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="43"/>
       <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="43"/>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="43"/>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -9535,7 +9535,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>23.8</v>
@@ -9735,7 +9735,7 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="46"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>88.4</v>
@@ -9929,13 +9929,13 @@
         <v>38</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>12.7</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -10252,13 +10252,13 @@
         <v>62</v>
       </c>
       <c r="C1" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="34" t="s">
         <v>148</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10296,37 +10296,37 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="52"/>
       <c r="B4" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
-        <v>151</v>
-      </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="52"/>
       <c r="B5" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -10436,19 +10436,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="55"/>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C14" s="16">
         <v>10</v>
@@ -10603,10 +10603,10 @@
         <v>25</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="29" t="s">
         <v>58</v>
@@ -10615,7 +10615,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="58"/>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C25">
         <v>51.4</v>
@@ -10770,7 +10770,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" s="29" t="s">
         <v>58</v>
@@ -10782,7 +10782,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="55"/>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C36">
         <v>10</v>
@@ -10962,7 +10962,7 @@
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="38"/>
       <c r="B52" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -10977,7 +10977,7 @@
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="38"/>
       <c r="B53" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>

</xml_diff>

<commit_message>
update some test coefficients
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E5FEB-FEFC-40AB-8984-656905A3EC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33358408-57E1-4794-90CB-9EAA16A6888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcox" sheetId="3" r:id="rId1"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="167">
   <si>
     <t>InitialN</t>
   </si>
@@ -794,6 +794,9 @@
   </si>
   <si>
     <t>None (Surface)</t>
+  </si>
+  <si>
+    <t>MidReproductive</t>
   </si>
 </sst>
 </file>
@@ -1661,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
@@ -9573,11 +9576,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27FB4FB-42CF-4046-81E6-EAE466E39234}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10165,7 +10168,7 @@
         <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More fine tuning of configs and coeffes.  Updating tests
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFC5E45-4D4C-4F12-B944-A599C7AE1D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE191A00-7F66-4340-AD72-D5A9CC4C2DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcox" sheetId="3" r:id="rId1"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="168">
   <si>
     <t>InitialN</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t>1-5Gra-B</t>
+  </si>
+  <si>
+    <t>Early harvest Potato Long (Group3)</t>
   </si>
 </sst>
 </file>
@@ -1664,8 +1667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2304,10 +2307,10 @@
         <v>44360</v>
       </c>
       <c r="F29" s="2">
-        <v>44682</v>
+        <v>44593</v>
       </c>
       <c r="G29" s="2">
-        <v>44986</v>
+        <v>44958</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2543,7 +2546,7 @@
         <v>44682</v>
       </c>
       <c r="F40" s="2">
-        <v>44986</v>
+        <v>44958</v>
       </c>
       <c r="G40" s="2">
         <v>45303</v>
@@ -3770,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AD42EA-A0EE-4986-A449-DEBA14E52DE4}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4762,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5361,7 +5364,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>64</v>
@@ -6031,8 +6034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDCA398-10B1-4DC3-A791-82E8FB2A1C43}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6444,7 +6447,7 @@
         <v>51</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -6461,8 +6464,8 @@
       <c r="E22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="17" t="s">
-        <v>56</v>
+      <c r="F22" s="16" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6579,7 +6582,7 @@
         <v>87</v>
       </c>
       <c r="E28" s="17">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="F28" s="17">
         <v>80</v>
@@ -6652,7 +6655,7 @@
         <v>51</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>33</v>
@@ -6670,7 +6673,7 @@
         <v>22</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>56</v>
+        <v>163</v>
       </c>
       <c r="F33" s="17" t="s">
         <v>22</v>
@@ -9577,10 +9580,10 @@
   <dimension ref="A1:R54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10015,7 +10018,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>147</v>
@@ -10529,10 +10532,10 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update test outputs to reflect variable soil N trigger
</commit_message>
<xml_diff>
--- a/TestComponents/TestSets/WS2/FieldConfigs.xlsx
+++ b/TestComponents/TestSets/WS2/FieldConfigs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\FieldNBalance\TestComponents\TestSets\WS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E4567D-59D6-46AE-AA61-3DF9B7307D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEEAB6F-8FC9-4098-A790-40C5A127E09E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{D68C7BAB-80DE-42A0-A5F7-D611BF3989D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Wilcox" sheetId="3" r:id="rId1"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="169">
   <si>
     <t>InitialN</t>
   </si>
@@ -800,6 +800,9 @@
   </si>
   <si>
     <t>Top30cm</t>
+  </si>
+  <si>
+    <t>Late</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050A90A1-2F9B-4EC2-8DA6-AD1920316E14}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7:G7"/>
     </sheetView>
   </sheetViews>
@@ -2760,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5455F7E-3498-453E-982D-C120B5675E13}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:F7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4765,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B8B917-5635-4965-8A45-89E9AEAAEA05}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5567,7 +5570,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>19</v>
@@ -6034,8 +6037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEDCA398-10B1-4DC3-A791-82E8FB2A1C43}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6315,7 +6318,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="17">
-        <v>74.099999999999994</v>
+        <v>63</v>
       </c>
       <c r="E14" s="17">
         <v>70.7</v>
@@ -6522,7 +6525,7 @@
         <v>137</v>
       </c>
       <c r="C25" s="17">
-        <v>74.099999999999994</v>
+        <v>63</v>
       </c>
       <c r="D25" s="17">
         <v>70.7</v>
@@ -6649,7 +6652,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>50</v>
@@ -6658,7 +6661,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -9583,7 +9586,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10162,7 +10165,7 @@
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="D32" t="s">
         <v>50</v>
@@ -10535,7 +10538,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7:E7"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>